<commit_message>
add i2c pull-ups and run outjobs
</commit_message>
<xml_diff>
--- a/bom/PurchaseList.xlsx
+++ b/bom/PurchaseList.xlsx
@@ -49,10 +49,10 @@
     <t>N-GLCD</t>
   </si>
   <si>
-    <t>07/12/2016</t>
-  </si>
-  <si>
-    <t>11:31:35</t>
+    <t>09/12/2016</t>
+  </si>
+  <si>
+    <t>12:14:28</t>
   </si>
   <si>
     <t>10</t>
@@ -67,7 +67,7 @@
     <t>LCD1</t>
   </si>
   <si>
-    <t>R1</t>
+    <t>R1, R2, R3</t>
   </si>
   <si>
     <t>U1</t>
@@ -1076,7 +1076,7 @@
         <v>54</v>
       </c>
       <c r="L2" s="10">
-        <v>388678</v>
+        <v>388668</v>
       </c>
       <c r="M2" s="49" t="s">
         <v>57</v>
@@ -1208,7 +1208,7 @@
         <v>54</v>
       </c>
       <c r="L4" s="10">
-        <v>1319395</v>
+        <v>1291554</v>
       </c>
       <c r="M4" s="49" t="s">
         <v>59</v>
@@ -1217,21 +1217,21 @@
         <v>1</v>
       </c>
       <c r="O4" s="10">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="P4" s="46">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="Q4" s="50">
         <f>ROUNDUP(P4*N4,0)</f>
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="R4" s="30">
         <v>4.1000000000000002E-2</v>
       </c>
       <c r="S4" s="30">
         <f>R4*Q4</f>
-        <v>0.41000000000000003</v>
+        <v>1.23</v>
       </c>
       <c r="T4" s="51">
         <f>ROW(T4) - ROW($A$1)</f>
@@ -1410,7 +1410,7 @@
       <c r="L8" s="14"/>
       <c r="M8" s="35">
         <f ca="1">NOW()</f>
-        <v>42711.480288541665</v>
+        <v>42713.510070717595</v>
       </c>
       <c r="N8" s="41"/>
       <c r="O8" s="15"/>
@@ -1421,11 +1421,11 @@
       </c>
       <c r="S8" s="37">
         <f>SUM(S2:S6)</f>
-        <v>26.43</v>
+        <v>27.25</v>
       </c>
       <c r="T8" s="45">
         <f>(SUM(S2:S6))/P9</f>
-        <v>2.6429999999999998</v>
+        <v>2.7250000000000001</v>
       </c>
     </row>
     <row r="9" spans="1:20" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">

</xml_diff>